<commit_message>
Restructuring the ml.py for displaying corectness of results
</commit_message>
<xml_diff>
--- a/Transavia/Production/Results/Results_daily_Abator_Bocsa.xlsx
+++ b/Transavia/Production/Results/Results_daily_Abator_Bocsa.xlsx
@@ -29,6 +29,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd.mm.yyyy"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -58,8 +61,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,7 +358,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -371,6 +375,1326 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>0.0111729446798563</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0.189994677901268</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0.4579775333404541</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>0.5095677971839905</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>0.5118885636329651</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>0.4800808131694794</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>0.3825526833534241</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>0.2239303141832352</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>0.1040439158678055</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>0.0004493343294598162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1">
+        <v>45256</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B32">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B33">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>0.0111729446798563</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B35">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>0.2737485468387604</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>0.4929396510124207</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B37">
+        <v>11</v>
+      </c>
+      <c r="C37">
+        <v>0.4965917468070984</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>0.52694171667099</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B39">
+        <v>13</v>
+      </c>
+      <c r="C39">
+        <v>0.4871638715267181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B40">
+        <v>14</v>
+      </c>
+      <c r="C40">
+        <v>0.2214532643556595</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B41">
+        <v>15</v>
+      </c>
+      <c r="C41">
+        <v>0.1607141345739365</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B42">
+        <v>16</v>
+      </c>
+      <c r="C42">
+        <v>0.1018696054816246</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B43">
+        <v>17</v>
+      </c>
+      <c r="C43">
+        <v>0.0004755306290462613</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B44">
+        <v>18</v>
+      </c>
+      <c r="C44">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B45">
+        <v>19</v>
+      </c>
+      <c r="C45">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B46">
+        <v>20</v>
+      </c>
+      <c r="C46">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B47">
+        <v>21</v>
+      </c>
+      <c r="C47">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B48">
+        <v>22</v>
+      </c>
+      <c r="C48">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="1">
+        <v>45257</v>
+      </c>
+      <c r="B49">
+        <v>23</v>
+      </c>
+      <c r="C49">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B58">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>0.000374900468159467</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B59">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <v>0.1691383868455887</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B60">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>0.2572034299373627</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B61">
+        <v>11</v>
+      </c>
+      <c r="C61">
+        <v>0.3297348916530609</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B62">
+        <v>12</v>
+      </c>
+      <c r="C62">
+        <v>0.3248184621334076</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B63">
+        <v>13</v>
+      </c>
+      <c r="C63">
+        <v>0.2669700980186462</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B64">
+        <v>14</v>
+      </c>
+      <c r="C64">
+        <v>0.1963153928518295</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B65">
+        <v>15</v>
+      </c>
+      <c r="C65">
+        <v>0.1733219474554062</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B66">
+        <v>16</v>
+      </c>
+      <c r="C66">
+        <v>0.1130970641970634</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B67">
+        <v>17</v>
+      </c>
+      <c r="C67">
+        <v>-0.001798878773115575</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B68">
+        <v>18</v>
+      </c>
+      <c r="C68">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B69">
+        <v>19</v>
+      </c>
+      <c r="C69">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B70">
+        <v>20</v>
+      </c>
+      <c r="C70">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B71">
+        <v>21</v>
+      </c>
+      <c r="C71">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B72">
+        <v>22</v>
+      </c>
+      <c r="C72">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="1">
+        <v>45258</v>
+      </c>
+      <c r="B73">
+        <v>23</v>
+      </c>
+      <c r="C73">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+      <c r="C74">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B78">
+        <v>4</v>
+      </c>
+      <c r="C78">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B79">
+        <v>5</v>
+      </c>
+      <c r="C79">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B80">
+        <v>6</v>
+      </c>
+      <c r="C80">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B81">
+        <v>7</v>
+      </c>
+      <c r="C81">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B82">
+        <v>8</v>
+      </c>
+      <c r="C82">
+        <v>0.000374900468159467</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B83">
+        <v>9</v>
+      </c>
+      <c r="C83">
+        <v>0.1560599356889725</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B84">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>0.2679129242897034</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B85">
+        <v>11</v>
+      </c>
+      <c r="C85">
+        <v>0.4149053692817688</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B86">
+        <v>12</v>
+      </c>
+      <c r="C86">
+        <v>0.4443180859088898</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B87">
+        <v>13</v>
+      </c>
+      <c r="C87">
+        <v>0.4521936178207397</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B88">
+        <v>14</v>
+      </c>
+      <c r="C88">
+        <v>0.3825526833534241</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B89">
+        <v>15</v>
+      </c>
+      <c r="C89">
+        <v>0.2233088463544846</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B90">
+        <v>16</v>
+      </c>
+      <c r="C90">
+        <v>0.1025843843817711</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B91">
+        <v>17</v>
+      </c>
+      <c r="C91">
+        <v>-0.001798878773115575</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B92">
+        <v>18</v>
+      </c>
+      <c r="C92">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B93">
+        <v>19</v>
+      </c>
+      <c r="C93">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B94">
+        <v>20</v>
+      </c>
+      <c r="C94">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B95">
+        <v>21</v>
+      </c>
+      <c r="C95">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B96">
+        <v>22</v>
+      </c>
+      <c r="C96">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" s="1">
+        <v>45259</v>
+      </c>
+      <c r="B97">
+        <v>23</v>
+      </c>
+      <c r="C97">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+      <c r="C98">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B99">
+        <v>1</v>
+      </c>
+      <c r="C99">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B100">
+        <v>2</v>
+      </c>
+      <c r="C100">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B101">
+        <v>3</v>
+      </c>
+      <c r="C101">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B102">
+        <v>4</v>
+      </c>
+      <c r="C102">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B103">
+        <v>5</v>
+      </c>
+      <c r="C103">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B104">
+        <v>6</v>
+      </c>
+      <c r="C104">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B105">
+        <v>7</v>
+      </c>
+      <c r="C105">
+        <v>0.0001293308450840414</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B106">
+        <v>8</v>
+      </c>
+      <c r="C106">
+        <v>0.000374900468159467</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B107">
+        <v>9</v>
+      </c>
+      <c r="C107">
+        <v>0.225534975528717</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B108">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>0.4751492440700531</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B109">
+        <v>11</v>
+      </c>
+      <c r="C109">
+        <v>0.5379148721694946</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B110">
+        <v>12</v>
+      </c>
+      <c r="C110">
+        <v>0.5444585680961609</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B111">
+        <v>13</v>
+      </c>
+      <c r="C111">
+        <v>0.4838798046112061</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B112">
+        <v>14</v>
+      </c>
+      <c r="C112">
+        <v>0.3951942622661591</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B113">
+        <v>15</v>
+      </c>
+      <c r="C113">
+        <v>0.2560143172740936</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B114">
+        <v>16</v>
+      </c>
+      <c r="C114">
+        <v>0.1139984130859375</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B115">
+        <v>17</v>
+      </c>
+      <c r="C115">
+        <v>0.0004493343294598162</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B116">
+        <v>18</v>
+      </c>
+      <c r="C116">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B117">
+        <v>19</v>
+      </c>
+      <c r="C117">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B118">
+        <v>20</v>
+      </c>
+      <c r="C118">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B119">
+        <v>21</v>
+      </c>
+      <c r="C119">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B120">
+        <v>22</v>
+      </c>
+      <c r="C120">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="1">
+        <v>45260</v>
+      </c>
+      <c r="B121">
+        <v>23</v>
+      </c>
+      <c r="C121">
+        <v>-0.0006825868622399867</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Deploying the Production Forecast for Transavia
</commit_message>
<xml_diff>
--- a/Transavia/Production/Results/Results_daily_Abator_Bocsa.xlsx
+++ b/Transavia/Production/Results/Results_daily_Abator_Bocsa.xlsx
@@ -358,7 +358,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C338"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,1322 +377,3709 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>45256</v>
+        <v>45364</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>0.0001293308450840414</v>
+        <v>0.3039960861206055</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>45256</v>
+        <v>45364</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C3">
-        <v>0.0001293308450840414</v>
+        <v>0.138564258813858</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>45256</v>
+        <v>45364</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C4">
-        <v>0.0001293308450840414</v>
+        <v>0.007687882520258427</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>45256</v>
+        <v>45364</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>45256</v>
+        <v>45364</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C6">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>45256</v>
+        <v>45364</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>45256</v>
+        <v>45364</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C8">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>45256</v>
+        <v>45364</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>45256</v>
+        <v>45364</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C10">
-        <v>0.0111729446798563</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0.189994677901268</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B12">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0.4579775333404541</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B13">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>0.5095677971839905</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C14">
-        <v>0.5118885636329651</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B15">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>0.4800808131694794</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>0.3825526833534241</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>0.2239303141832352</v>
+        <v>0.1531635969877243</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B18">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>0.1040439158678055</v>
+        <v>0.2864326238632202</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B19">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>0.0004493343294598162</v>
+        <v>0.3269355893135071</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B20">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>-0.0006825868622399867</v>
+        <v>0.342717707157135</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>-0.0006825868622399867</v>
+        <v>0.5333595275878906</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B22">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C22">
-        <v>-0.0006825868622399867</v>
+        <v>0.6083981990814209</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B23">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>-0.0006825868622399867</v>
+        <v>0.5802819132804871</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B24">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>-0.0006825868622399867</v>
+        <v>0.5956315994262695</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1">
-        <v>45256</v>
+        <v>45365</v>
       </c>
       <c r="B25">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C25">
-        <v>-0.0006825868622399867</v>
+        <v>0.4815758168697357</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1">
-        <v>45257</v>
+        <v>45365</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C26">
-        <v>0.0001293308450840414</v>
+        <v>0.3294726014137268</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1">
-        <v>45257</v>
+        <v>45365</v>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C27">
-        <v>0.0001293308450840414</v>
+        <v>0.1639994531869888</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1">
-        <v>45257</v>
+        <v>45365</v>
       </c>
       <c r="B28">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C28">
-        <v>0.0001293308450840414</v>
+        <v>0.008538169786334038</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1">
-        <v>45257</v>
+        <v>45365</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C29">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1">
-        <v>45257</v>
+        <v>45365</v>
       </c>
       <c r="B30">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C30">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1">
-        <v>45257</v>
+        <v>45365</v>
       </c>
       <c r="B31">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C31">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1">
-        <v>45257</v>
+        <v>45365</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C32">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1">
-        <v>45257</v>
+        <v>45365</v>
       </c>
       <c r="B33">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C33">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1">
-        <v>45257</v>
+        <v>45365</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C34">
-        <v>0.0111729446798563</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C35">
-        <v>0.2737485468387604</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B36">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <v>0.4929396510124207</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B37">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C37">
-        <v>0.4965917468070984</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B38">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C38">
-        <v>0.52694171667099</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B39">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C39">
-        <v>0.4871638715267181</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B40">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C40">
-        <v>0.2214532643556595</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B41">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C41">
-        <v>0.1607141345739365</v>
+        <v>0.2028349190950394</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B42">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>0.1018696054816246</v>
+        <v>0.3505081832408905</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B43">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C43">
-        <v>0.0004755306290462613</v>
+        <v>0.3678479492664337</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B44">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>-0.0006825868622399867</v>
+        <v>0.4498375952243805</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B45">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C45">
-        <v>-0.0006825868622399867</v>
+        <v>0.6469483971595764</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B46">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C46">
-        <v>-0.0006825868622399867</v>
+        <v>0.6009387373924255</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B47">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C47">
-        <v>-0.0006825868622399867</v>
+        <v>0.6074647903442383</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B48">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C48">
-        <v>-0.0006825868622399867</v>
+        <v>0.6316176652908325</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1">
-        <v>45257</v>
+        <v>45366</v>
       </c>
       <c r="B49">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C49">
-        <v>-0.0006825868622399867</v>
+        <v>0.5226923823356628</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1">
-        <v>45258</v>
+        <v>45366</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C50">
-        <v>0.0001293308450840414</v>
+        <v>0.4252724945545197</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1">
-        <v>45258</v>
+        <v>45366</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>0.0001293308450840414</v>
+        <v>0.1775433868169785</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1">
-        <v>45258</v>
+        <v>45366</v>
       </c>
       <c r="B52">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C52">
-        <v>0.0001293308450840414</v>
+        <v>0.01243957597762346</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1">
-        <v>45258</v>
+        <v>45366</v>
       </c>
       <c r="B53">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C53">
-        <v>0.0001293308450840414</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1">
-        <v>45258</v>
+        <v>45366</v>
       </c>
       <c r="B54">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C54">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1">
-        <v>45258</v>
+        <v>45366</v>
       </c>
       <c r="B55">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C55">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1">
-        <v>45258</v>
+        <v>45366</v>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C56">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1">
-        <v>45258</v>
+        <v>45366</v>
       </c>
       <c r="B57">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C57">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1">
-        <v>45258</v>
+        <v>45366</v>
       </c>
       <c r="B58">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C58">
-        <v>0.000374900468159467</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B59">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>0.1691383868455887</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B60">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C60">
-        <v>0.2572034299373627</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B61">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C61">
-        <v>0.3297348916530609</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B62">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>0.3248184621334076</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B63">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C63">
-        <v>0.2669700980186462</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B64">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C64">
-        <v>0.1963153928518295</v>
+        <v>0.01354346703737974</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B65">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C65">
-        <v>0.1733219474554062</v>
+        <v>0.203892782330513</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B66">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C66">
-        <v>0.1130970641970634</v>
+        <v>0.3538053929805756</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B67">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C67">
-        <v>-0.001798878773115575</v>
+        <v>0.381721556186676</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B68">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C68">
-        <v>-0.0006825868622399867</v>
+        <v>0.4433241784572601</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B69">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C69">
-        <v>-0.0006825868622399867</v>
+        <v>0.6273519396781921</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B70">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C70">
-        <v>-0.0006825868622399867</v>
+        <v>0.6669963598251343</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B71">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C71">
-        <v>-0.0006825868622399867</v>
+        <v>0.6575444340705872</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B72">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C72">
-        <v>-0.0006825868622399867</v>
+        <v>0.6338027715682983</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="1">
-        <v>45258</v>
+        <v>45367</v>
       </c>
       <c r="B73">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C73">
-        <v>-0.0006825868622399867</v>
+        <v>0.5384136438369751</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1">
-        <v>45259</v>
+        <v>45367</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C74">
-        <v>0.0001293308450840414</v>
+        <v>0.472400575876236</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="1">
-        <v>45259</v>
+        <v>45367</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C75">
-        <v>0.0001293308450840414</v>
+        <v>0.2025753557682037</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1">
-        <v>45259</v>
+        <v>45367</v>
       </c>
       <c r="B76">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C76">
-        <v>0.0001293308450840414</v>
+        <v>0.01743231527507305</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="1">
-        <v>45259</v>
+        <v>45367</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C77">
-        <v>0.0001293308450840414</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="1">
-        <v>45259</v>
+        <v>45367</v>
       </c>
       <c r="B78">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C78">
-        <v>0.0001293308450840414</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="1">
-        <v>45259</v>
+        <v>45367</v>
       </c>
       <c r="B79">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C79">
-        <v>0.0001293308450840414</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="1">
-        <v>45259</v>
+        <v>45367</v>
       </c>
       <c r="B80">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C80">
-        <v>0.0001293308450840414</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="1">
-        <v>45259</v>
+        <v>45367</v>
       </c>
       <c r="B81">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C81">
-        <v>0.0001293308450840414</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="1">
-        <v>45259</v>
+        <v>45367</v>
       </c>
       <c r="B82">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C82">
-        <v>0.000374900468159467</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B83">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C83">
-        <v>0.1560599356889725</v>
+        <v>0.001873338012956083</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B84">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C84">
-        <v>0.2679129242897034</v>
+        <v>0.001873338012956083</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B85">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C85">
-        <v>0.4149053692817688</v>
+        <v>0.001873338012956083</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B86">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C86">
-        <v>0.4443180859088898</v>
+        <v>0.001873338012956083</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B87">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C87">
-        <v>0.4521936178207397</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B88">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C88">
-        <v>0.3825526833534241</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B89">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C89">
-        <v>0.2233088463544846</v>
+        <v>0.1169179677963257</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B90">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C90">
-        <v>0.1025843843817711</v>
+        <v>0.2180894762277603</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B91">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C91">
-        <v>-0.001798878773115575</v>
+        <v>0.3768282532691956</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B92">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C92">
-        <v>-0.0006825868622399867</v>
+        <v>0.5186205506324768</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B93">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C93">
-        <v>-0.0006825868622399867</v>
+        <v>0.6430674195289612</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B94">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C94">
-        <v>-0.0006825868622399867</v>
+        <v>0.6727409362792969</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B95">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C95">
-        <v>-0.0006825868622399867</v>
+        <v>0.6742448806762695</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B96">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C96">
-        <v>-0.0006825868622399867</v>
+        <v>0.6349566578865051</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="1">
-        <v>45259</v>
+        <v>45368</v>
       </c>
       <c r="B97">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C97">
-        <v>-0.0006825868622399867</v>
+        <v>0.5490165948867798</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="1">
-        <v>45260</v>
+        <v>45368</v>
       </c>
       <c r="B98">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C98">
-        <v>0.0001293308450840414</v>
+        <v>0.443498969078064</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="1">
-        <v>45260</v>
+        <v>45368</v>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C99">
-        <v>0.0001293308450840414</v>
+        <v>0.1606403440237045</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="1">
-        <v>45260</v>
+        <v>45368</v>
       </c>
       <c r="B100">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C100">
-        <v>0.0001293308450840414</v>
+        <v>0.009733018465340137</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1">
-        <v>45260</v>
+        <v>45368</v>
       </c>
       <c r="B101">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="C101">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="1">
-        <v>45260</v>
+        <v>45368</v>
       </c>
       <c r="B102">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C102">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="1">
-        <v>45260</v>
+        <v>45368</v>
       </c>
       <c r="B103">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C103">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="1">
-        <v>45260</v>
+        <v>45368</v>
       </c>
       <c r="B104">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C104">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="1">
-        <v>45260</v>
+        <v>45368</v>
       </c>
       <c r="B105">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C105">
-        <v>0.0001293308450840414</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="1">
-        <v>45260</v>
+        <v>45368</v>
       </c>
       <c r="B106">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="C106">
-        <v>0.000374900468159467</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B107">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C107">
-        <v>0.225534975528717</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B108">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C108">
-        <v>0.4751492440700531</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B109">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C109">
-        <v>0.5379148721694946</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B110">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C110">
-        <v>0.5444585680961609</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B111">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C111">
-        <v>0.4838798046112061</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B112">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C112">
-        <v>0.3951942622661591</v>
+        <v>0.01375892665237188</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B113">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C113">
-        <v>0.2560143172740936</v>
+        <v>0.219965010881424</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B114">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C114">
-        <v>0.1139984130859375</v>
+        <v>0.3492618501186371</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B115">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C115">
-        <v>0.0004493343294598162</v>
+        <v>0.3729380369186401</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B116">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C116">
-        <v>-0.0006825868622399867</v>
+        <v>0.414051741361618</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B117">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C117">
-        <v>-0.0006825868622399867</v>
+        <v>0.4409171342849731</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B118">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C118">
-        <v>-0.0006825868622399867</v>
+        <v>0.5409641861915588</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B119">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C119">
-        <v>-0.0006825868622399867</v>
+        <v>0.5497909784317017</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B120">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C120">
-        <v>-0.0006825868622399867</v>
+        <v>0.5241569876670837</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="1">
-        <v>45260</v>
+        <v>45369</v>
       </c>
       <c r="B121">
+        <v>14</v>
+      </c>
+      <c r="C121">
+        <v>0.5577781796455383</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B122">
+        <v>15</v>
+      </c>
+      <c r="C122">
+        <v>0.4442236423492432</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B123">
+        <v>16</v>
+      </c>
+      <c r="C123">
+        <v>0.2170901447534561</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B124">
+        <v>17</v>
+      </c>
+      <c r="C124">
+        <v>0.02100068144500256</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B125">
+        <v>18</v>
+      </c>
+      <c r="C125">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B126">
+        <v>19</v>
+      </c>
+      <c r="C126">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B127">
+        <v>20</v>
+      </c>
+      <c r="C127">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B128">
+        <v>21</v>
+      </c>
+      <c r="C128">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B129">
+        <v>22</v>
+      </c>
+      <c r="C129">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" s="1">
+        <v>45369</v>
+      </c>
+      <c r="B130">
         <v>23</v>
       </c>
-      <c r="C121">
-        <v>-0.0006825868622399867</v>
+      <c r="C130">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+      <c r="C131">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B132">
+        <v>1</v>
+      </c>
+      <c r="C132">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B133">
+        <v>2</v>
+      </c>
+      <c r="C133">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B134">
+        <v>3</v>
+      </c>
+      <c r="C134">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B135">
+        <v>4</v>
+      </c>
+      <c r="C135">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B136">
+        <v>5</v>
+      </c>
+      <c r="C136">
+        <v>0.01375892665237188</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B137">
+        <v>6</v>
+      </c>
+      <c r="C137">
+        <v>0.1554246991872787</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B138">
+        <v>7</v>
+      </c>
+      <c r="C138">
+        <v>0.2826413214206696</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B139">
+        <v>8</v>
+      </c>
+      <c r="C139">
+        <v>0.3504942953586578</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B140">
+        <v>9</v>
+      </c>
+      <c r="C140">
+        <v>0.4736542999744415</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B141">
+        <v>10</v>
+      </c>
+      <c r="C141">
+        <v>0.6175188422203064</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B142">
+        <v>11</v>
+      </c>
+      <c r="C142">
+        <v>0.55228191614151</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B143">
+        <v>12</v>
+      </c>
+      <c r="C143">
+        <v>0.77106773853302</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B144">
+        <v>13</v>
+      </c>
+      <c r="C144">
+        <v>0.7280515432357788</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B145">
+        <v>14</v>
+      </c>
+      <c r="C145">
+        <v>0.6689601540565491</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B146">
+        <v>15</v>
+      </c>
+      <c r="C146">
+        <v>0.5792936682701111</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B147">
+        <v>16</v>
+      </c>
+      <c r="C147">
+        <v>0.3157016336917877</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B148">
+        <v>17</v>
+      </c>
+      <c r="C148">
+        <v>0.02100843377411366</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B149">
+        <v>18</v>
+      </c>
+      <c r="C149">
+        <v>0.005535293836146593</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B150">
+        <v>19</v>
+      </c>
+      <c r="C150">
+        <v>0.00233306479640305</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B151">
+        <v>20</v>
+      </c>
+      <c r="C151">
+        <v>0.00233306479640305</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B152">
+        <v>21</v>
+      </c>
+      <c r="C152">
+        <v>0.00233306479640305</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B153">
+        <v>22</v>
+      </c>
+      <c r="C153">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" s="1">
+        <v>45370</v>
+      </c>
+      <c r="B154">
+        <v>23</v>
+      </c>
+      <c r="C154">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B155">
+        <v>0</v>
+      </c>
+      <c r="C155">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="C156">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B157">
+        <v>2</v>
+      </c>
+      <c r="C157">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B158">
+        <v>3</v>
+      </c>
+      <c r="C158">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B159">
+        <v>4</v>
+      </c>
+      <c r="C159">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B160">
+        <v>5</v>
+      </c>
+      <c r="C160">
+        <v>0.0144943306222558</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B161">
+        <v>6</v>
+      </c>
+      <c r="C161">
+        <v>0.1657159030437469</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B162">
+        <v>7</v>
+      </c>
+      <c r="C162">
+        <v>0.3122064471244812</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B163">
+        <v>8</v>
+      </c>
+      <c r="C163">
+        <v>0.3471722900867462</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B164">
+        <v>9</v>
+      </c>
+      <c r="C164">
+        <v>0.502892792224884</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B165">
+        <v>10</v>
+      </c>
+      <c r="C165">
+        <v>0.5648559927940369</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B166">
+        <v>11</v>
+      </c>
+      <c r="C166">
+        <v>0.7599678635597229</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B167">
+        <v>12</v>
+      </c>
+      <c r="C167">
+        <v>0.7935822010040283</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B168">
+        <v>13</v>
+      </c>
+      <c r="C168">
+        <v>0.8243045210838318</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B169">
+        <v>14</v>
+      </c>
+      <c r="C169">
+        <v>0.7576906085014343</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B170">
+        <v>15</v>
+      </c>
+      <c r="C170">
+        <v>0.614687979221344</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B171">
+        <v>16</v>
+      </c>
+      <c r="C171">
+        <v>0.3211678862571716</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B172">
+        <v>17</v>
+      </c>
+      <c r="C172">
+        <v>0.02528130449354649</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B173">
+        <v>18</v>
+      </c>
+      <c r="C173">
+        <v>0.004636262077838182</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B174">
+        <v>19</v>
+      </c>
+      <c r="C174">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B175">
+        <v>20</v>
+      </c>
+      <c r="C175">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B176">
+        <v>21</v>
+      </c>
+      <c r="C176">
+        <v>0.001822930993512273</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B177">
+        <v>22</v>
+      </c>
+      <c r="C177">
+        <v>0.001822930993512273</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3">
+      <c r="A178" s="1">
+        <v>45371</v>
+      </c>
+      <c r="B178">
+        <v>23</v>
+      </c>
+      <c r="C178">
+        <v>0.001822930993512273</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3">
+      <c r="A180" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B180">
+        <v>1</v>
+      </c>
+      <c r="C180">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3">
+      <c r="A181" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B181">
+        <v>2</v>
+      </c>
+      <c r="C181">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B182">
+        <v>3</v>
+      </c>
+      <c r="C182">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B183">
+        <v>4</v>
+      </c>
+      <c r="C183">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B184">
+        <v>5</v>
+      </c>
+      <c r="C184">
+        <v>0.04279576241970062</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3">
+      <c r="A185" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B185">
+        <v>6</v>
+      </c>
+      <c r="C185">
+        <v>0.2264294177293777</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B186">
+        <v>7</v>
+      </c>
+      <c r="C186">
+        <v>0.3320692181587219</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B187">
+        <v>8</v>
+      </c>
+      <c r="C187">
+        <v>0.3862507045269012</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B188">
+        <v>9</v>
+      </c>
+      <c r="C188">
+        <v>0.447108268737793</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
+      <c r="A189" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B189">
+        <v>10</v>
+      </c>
+      <c r="C189">
+        <v>0.7802374362945557</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B190">
+        <v>11</v>
+      </c>
+      <c r="C190">
+        <v>0.821527898311615</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3">
+      <c r="A191" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B191">
+        <v>12</v>
+      </c>
+      <c r="C191">
+        <v>0.8387635946273804</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B192">
+        <v>13</v>
+      </c>
+      <c r="C192">
+        <v>0.7663832902908325</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B193">
+        <v>14</v>
+      </c>
+      <c r="C193">
+        <v>0.6836625933647156</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3">
+      <c r="A194" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B194">
+        <v>15</v>
+      </c>
+      <c r="C194">
+        <v>0.6602174639701843</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3">
+      <c r="A195" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B195">
+        <v>16</v>
+      </c>
+      <c r="C195">
+        <v>0.3830647766590118</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3">
+      <c r="A196" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B196">
+        <v>17</v>
+      </c>
+      <c r="C196">
+        <v>0.02511965297162533</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B197">
+        <v>18</v>
+      </c>
+      <c r="C197">
+        <v>0.004636262077838182</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B198">
+        <v>19</v>
+      </c>
+      <c r="C198">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B199">
+        <v>20</v>
+      </c>
+      <c r="C199">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B200">
+        <v>21</v>
+      </c>
+      <c r="C200">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B201">
+        <v>22</v>
+      </c>
+      <c r="C201">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3">
+      <c r="A202" s="1">
+        <v>45372</v>
+      </c>
+      <c r="B202">
+        <v>23</v>
+      </c>
+      <c r="C202">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B203">
+        <v>0</v>
+      </c>
+      <c r="C203">
+        <v>0.002426850143820047</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B204">
+        <v>1</v>
+      </c>
+      <c r="C204">
+        <v>0.002426850143820047</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3">
+      <c r="A205" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B205">
+        <v>2</v>
+      </c>
+      <c r="C205">
+        <v>0.002426850143820047</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B206">
+        <v>3</v>
+      </c>
+      <c r="C206">
+        <v>0.002676395466551185</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3">
+      <c r="A207" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B207">
+        <v>4</v>
+      </c>
+      <c r="C207">
+        <v>0.002676395466551185</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3">
+      <c r="A208" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B208">
+        <v>5</v>
+      </c>
+      <c r="C208">
+        <v>0.04334927350282669</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B209">
+        <v>6</v>
+      </c>
+      <c r="C209">
+        <v>0.201739564538002</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3">
+      <c r="A210" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B210">
+        <v>7</v>
+      </c>
+      <c r="C210">
+        <v>0.3197154104709625</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3">
+      <c r="A211" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B211">
+        <v>8</v>
+      </c>
+      <c r="C211">
+        <v>0.3832141160964966</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B212">
+        <v>9</v>
+      </c>
+      <c r="C212">
+        <v>0.4454418122768402</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B213">
+        <v>10</v>
+      </c>
+      <c r="C213">
+        <v>0.6977189779281616</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B214">
+        <v>11</v>
+      </c>
+      <c r="C214">
+        <v>0.7818703055381775</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B215">
+        <v>12</v>
+      </c>
+      <c r="C215">
+        <v>0.7823619246482849</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B216">
+        <v>13</v>
+      </c>
+      <c r="C216">
+        <v>0.9103758931159973</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B217">
+        <v>14</v>
+      </c>
+      <c r="C217">
+        <v>0.7971689701080322</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B218">
+        <v>15</v>
+      </c>
+      <c r="C218">
+        <v>0.7029615044593811</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B219">
+        <v>16</v>
+      </c>
+      <c r="C219">
+        <v>0.511029839515686</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B220">
+        <v>17</v>
+      </c>
+      <c r="C220">
+        <v>0.03001339919865131</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B221">
+        <v>18</v>
+      </c>
+      <c r="C221">
+        <v>0.006026065442711115</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B222">
+        <v>19</v>
+      </c>
+      <c r="C222">
+        <v>-0.001574540045112371</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B223">
+        <v>20</v>
+      </c>
+      <c r="C223">
+        <v>-0.001574540045112371</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B224">
+        <v>21</v>
+      </c>
+      <c r="C224">
+        <v>-0.003064034273847938</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B225">
+        <v>22</v>
+      </c>
+      <c r="C225">
+        <v>-0.003064034273847938</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" s="1">
+        <v>45373</v>
+      </c>
+      <c r="B226">
+        <v>23</v>
+      </c>
+      <c r="C226">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3">
+      <c r="A227" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B227">
+        <v>0</v>
+      </c>
+      <c r="C227">
+        <v>0.002426850143820047</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B228">
+        <v>1</v>
+      </c>
+      <c r="C228">
+        <v>0.002426850143820047</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B229">
+        <v>2</v>
+      </c>
+      <c r="C229">
+        <v>0.002426850143820047</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B230">
+        <v>3</v>
+      </c>
+      <c r="C230">
+        <v>0.002676395466551185</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B231">
+        <v>4</v>
+      </c>
+      <c r="C231">
+        <v>0.002936984179541469</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B232">
+        <v>5</v>
+      </c>
+      <c r="C232">
+        <v>0.03597201034426689</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B233">
+        <v>6</v>
+      </c>
+      <c r="C233">
+        <v>0.1678444594144821</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B234">
+        <v>7</v>
+      </c>
+      <c r="C234">
+        <v>0.2831286489963531</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B235">
+        <v>8</v>
+      </c>
+      <c r="C235">
+        <v>0.3570091128349304</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B236">
+        <v>9</v>
+      </c>
+      <c r="C236">
+        <v>0.5389638543128967</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3">
+      <c r="A237" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B237">
+        <v>10</v>
+      </c>
+      <c r="C237">
+        <v>0.7659305930137634</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B238">
+        <v>11</v>
+      </c>
+      <c r="C238">
+        <v>0.838615894317627</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3">
+      <c r="A239" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B239">
+        <v>12</v>
+      </c>
+      <c r="C239">
+        <v>0.8198053240776062</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B240">
+        <v>13</v>
+      </c>
+      <c r="C240">
+        <v>0.840302050113678</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B241">
+        <v>14</v>
+      </c>
+      <c r="C241">
+        <v>0.7809241414070129</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3">
+      <c r="A242" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B242">
+        <v>15</v>
+      </c>
+      <c r="C242">
+        <v>0.563556432723999</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B243">
+        <v>16</v>
+      </c>
+      <c r="C243">
+        <v>0.3210353851318359</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3">
+      <c r="A244" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B244">
+        <v>17</v>
+      </c>
+      <c r="C244">
+        <v>0.02221535332500935</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3">
+      <c r="A245" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B245">
+        <v>18</v>
+      </c>
+      <c r="C245">
+        <v>0.004636262077838182</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3">
+      <c r="A246" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B246">
+        <v>19</v>
+      </c>
+      <c r="C246">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B247">
+        <v>20</v>
+      </c>
+      <c r="C247">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B248">
+        <v>21</v>
+      </c>
+      <c r="C248">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3">
+      <c r="A249" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B249">
+        <v>22</v>
+      </c>
+      <c r="C249">
+        <v>0.002071057911962271</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" s="1">
+        <v>45374</v>
+      </c>
+      <c r="B250">
+        <v>23</v>
+      </c>
+      <c r="C250">
+        <v>0.002071057911962271</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B251">
+        <v>0</v>
+      </c>
+      <c r="C251">
+        <v>0.003186529269441962</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B252">
+        <v>1</v>
+      </c>
+      <c r="C252">
+        <v>0.003186529269441962</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3">
+      <c r="A253" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B253">
+        <v>2</v>
+      </c>
+      <c r="C253">
+        <v>0.003186529269441962</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B254">
+        <v>3</v>
+      </c>
+      <c r="C254">
+        <v>0.003186529269441962</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B255">
+        <v>4</v>
+      </c>
+      <c r="C255">
+        <v>0.003186529269441962</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3">
+      <c r="A256" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B256">
+        <v>5</v>
+      </c>
+      <c r="C256">
+        <v>0.03793659061193466</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B257">
+        <v>6</v>
+      </c>
+      <c r="C257">
+        <v>0.1589391231536865</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B258">
+        <v>7</v>
+      </c>
+      <c r="C258">
+        <v>0.2691071033477783</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3">
+      <c r="A259" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B259">
+        <v>8</v>
+      </c>
+      <c r="C259">
+        <v>0.3982172310352325</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3">
+      <c r="A260" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B260">
+        <v>9</v>
+      </c>
+      <c r="C260">
+        <v>0.5408667325973511</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3">
+      <c r="A261" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B261">
+        <v>10</v>
+      </c>
+      <c r="C261">
+        <v>0.6022312045097351</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3">
+      <c r="A262" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B262">
+        <v>11</v>
+      </c>
+      <c r="C262">
+        <v>0.7723228335380554</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B263">
+        <v>12</v>
+      </c>
+      <c r="C263">
+        <v>0.7553914785385132</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B264">
+        <v>13</v>
+      </c>
+      <c r="C264">
+        <v>0.780234158039093</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3">
+      <c r="A265" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B265">
+        <v>14</v>
+      </c>
+      <c r="C265">
+        <v>0.6081504821777344</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B266">
+        <v>15</v>
+      </c>
+      <c r="C266">
+        <v>0.5824326872825623</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B267">
+        <v>16</v>
+      </c>
+      <c r="C267">
+        <v>0.3905293047428131</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B268">
+        <v>17</v>
+      </c>
+      <c r="C268">
+        <v>0.02817033790051937</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3">
+      <c r="A269" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B269">
+        <v>18</v>
+      </c>
+      <c r="C269">
+        <v>0.005025160033255816</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B270">
+        <v>19</v>
+      </c>
+      <c r="C270">
+        <v>0.001560923759825528</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B271">
+        <v>20</v>
+      </c>
+      <c r="C271">
+        <v>0.00233306479640305</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B272">
+        <v>21</v>
+      </c>
+      <c r="C272">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B273">
+        <v>22</v>
+      </c>
+      <c r="C273">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" s="1">
+        <v>45375</v>
+      </c>
+      <c r="B274">
+        <v>23</v>
+      </c>
+      <c r="C274">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3">
+      <c r="A275" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B275">
+        <v>0</v>
+      </c>
+      <c r="C275">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B276">
+        <v>1</v>
+      </c>
+      <c r="C276">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B277">
+        <v>2</v>
+      </c>
+      <c r="C277">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3">
+      <c r="A278" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B278">
+        <v>3</v>
+      </c>
+      <c r="C278">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B279">
+        <v>4</v>
+      </c>
+      <c r="C279">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B280">
+        <v>5</v>
+      </c>
+      <c r="C280">
+        <v>0.08701945096254349</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3">
+      <c r="A281" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B281">
+        <v>6</v>
+      </c>
+      <c r="C281">
+        <v>0.296549379825592</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3">
+      <c r="A282" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B282">
+        <v>7</v>
+      </c>
+      <c r="C282">
+        <v>0.3118192553520203</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3">
+      <c r="A283" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B283">
+        <v>8</v>
+      </c>
+      <c r="C283">
+        <v>0.2224577516317368</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3">
+      <c r="A284" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B284">
+        <v>9</v>
+      </c>
+      <c r="C284">
+        <v>0.4194476008415222</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3">
+      <c r="A285" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B285">
+        <v>10</v>
+      </c>
+      <c r="C285">
+        <v>0.5621249675750732</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3">
+      <c r="A286" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B286">
+        <v>11</v>
+      </c>
+      <c r="C286">
+        <v>0.6006543636322021</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B287">
+        <v>12</v>
+      </c>
+      <c r="C287">
+        <v>0.7866647839546204</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B288">
+        <v>13</v>
+      </c>
+      <c r="C288">
+        <v>0.7469737529754639</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B289">
+        <v>14</v>
+      </c>
+      <c r="C289">
+        <v>0.7285200357437134</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B290">
+        <v>15</v>
+      </c>
+      <c r="C290">
+        <v>0.6659958958625793</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B291">
+        <v>16</v>
+      </c>
+      <c r="C291">
+        <v>0.4039880335330963</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B292">
+        <v>17</v>
+      </c>
+      <c r="C292">
+        <v>0.03032158501446247</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B293">
+        <v>18</v>
+      </c>
+      <c r="C293">
+        <v>0.005025160033255816</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3">
+      <c r="A294" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B294">
+        <v>19</v>
+      </c>
+      <c r="C294">
+        <v>0.001822930993512273</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B295">
+        <v>20</v>
+      </c>
+      <c r="C295">
+        <v>0.001822930993512273</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B296">
+        <v>21</v>
+      </c>
+      <c r="C296">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B297">
+        <v>22</v>
+      </c>
+      <c r="C297">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" s="1">
+        <v>45376</v>
+      </c>
+      <c r="B298">
+        <v>23</v>
+      </c>
+      <c r="C298">
+        <v>0.001019873307086527</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3">
+      <c r="A299" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B299">
+        <v>0</v>
+      </c>
+      <c r="C299">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3">
+      <c r="A300" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B300">
+        <v>1</v>
+      </c>
+      <c r="C300">
+        <v>0.001873338012956083</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3">
+      <c r="A301" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B301">
+        <v>2</v>
+      </c>
+      <c r="C301">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3">
+      <c r="A302" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B302">
+        <v>3</v>
+      </c>
+      <c r="C302">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3">
+      <c r="A303" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B303">
+        <v>4</v>
+      </c>
+      <c r="C303">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3">
+      <c r="A304" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B304">
+        <v>5</v>
+      </c>
+      <c r="C304">
+        <v>0.04206036403775215</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3">
+      <c r="A305" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B305">
+        <v>6</v>
+      </c>
+      <c r="C305">
+        <v>0.181069627404213</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="A306" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B306">
+        <v>7</v>
+      </c>
+      <c r="C306">
+        <v>0.3110060691833496</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3">
+      <c r="A307" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B307">
+        <v>8</v>
+      </c>
+      <c r="C307">
+        <v>0.3256857991218567</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3">
+      <c r="A308" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B308">
+        <v>9</v>
+      </c>
+      <c r="C308">
+        <v>0.4600401222705841</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3">
+      <c r="A309" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B309">
+        <v>10</v>
+      </c>
+      <c r="C309">
+        <v>0.5852345824241638</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3">
+      <c r="A310" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B310">
+        <v>11</v>
+      </c>
+      <c r="C310">
+        <v>0.5273016095161438</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3">
+      <c r="A311" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B311">
+        <v>12</v>
+      </c>
+      <c r="C311">
+        <v>0.6154138445854187</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3">
+      <c r="A312" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B312">
+        <v>13</v>
+      </c>
+      <c r="C312">
+        <v>0.6494281888008118</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3">
+      <c r="A313" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B313">
+        <v>14</v>
+      </c>
+      <c r="C313">
+        <v>0.5516771674156189</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3">
+      <c r="A314" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B314">
+        <v>15</v>
+      </c>
+      <c r="C314">
+        <v>0.4223678410053253</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3">
+      <c r="A315" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B315">
+        <v>16</v>
+      </c>
+      <c r="C315">
+        <v>0.1634838283061981</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3">
+      <c r="A316" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B316">
+        <v>17</v>
+      </c>
+      <c r="C316">
+        <v>0.009733018465340137</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3">
+      <c r="A317" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B317">
+        <v>18</v>
+      </c>
+      <c r="C317">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3">
+      <c r="A318" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B318">
+        <v>19</v>
+      </c>
+      <c r="C318">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3">
+      <c r="A319" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B319">
+        <v>20</v>
+      </c>
+      <c r="C319">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3">
+      <c r="A320" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B320">
+        <v>21</v>
+      </c>
+      <c r="C320">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3">
+      <c r="A321" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B321">
+        <v>22</v>
+      </c>
+      <c r="C321">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="322" spans="1:3">
+      <c r="A322" s="1">
+        <v>45377</v>
+      </c>
+      <c r="B322">
+        <v>23</v>
+      </c>
+      <c r="C322">
+        <v>0.0006087372894398868</v>
+      </c>
+    </row>
+    <row r="323" spans="1:3">
+      <c r="A323" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B323">
+        <v>0</v>
+      </c>
+      <c r="C323">
+        <v>0.001462202053517103</v>
+      </c>
+    </row>
+    <row r="324" spans="1:3">
+      <c r="A324" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B324">
+        <v>1</v>
+      </c>
+      <c r="C324">
+        <v>0.001190799288451672</v>
+      </c>
+    </row>
+    <row r="325" spans="1:3">
+      <c r="A325" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B325">
+        <v>2</v>
+      </c>
+      <c r="C325">
+        <v>0.001190799288451672</v>
+      </c>
+    </row>
+    <row r="326" spans="1:3">
+      <c r="A326" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B326">
+        <v>3</v>
+      </c>
+      <c r="C326">
+        <v>0.001190799288451672</v>
+      </c>
+    </row>
+    <row r="327" spans="1:3">
+      <c r="A327" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B327">
+        <v>4</v>
+      </c>
+      <c r="C327">
+        <v>0.001190799288451672</v>
+      </c>
+    </row>
+    <row r="328" spans="1:3">
+      <c r="A328" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B328">
+        <v>5</v>
+      </c>
+      <c r="C328">
+        <v>0.08555274456739426</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3">
+      <c r="A329" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B329">
+        <v>6</v>
+      </c>
+      <c r="C329">
+        <v>0.2255028635263443</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3">
+      <c r="A330" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B330">
+        <v>7</v>
+      </c>
+      <c r="C330">
+        <v>0.3339379131793976</v>
+      </c>
+    </row>
+    <row r="331" spans="1:3">
+      <c r="A331" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B331">
+        <v>8</v>
+      </c>
+      <c r="C331">
+        <v>0.2840148508548737</v>
+      </c>
+    </row>
+    <row r="332" spans="1:3">
+      <c r="A332" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B332">
+        <v>9</v>
+      </c>
+      <c r="C332">
+        <v>0.609189510345459</v>
+      </c>
+    </row>
+    <row r="333" spans="1:3">
+      <c r="A333" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B333">
+        <v>10</v>
+      </c>
+      <c r="C333">
+        <v>0.6064830422401428</v>
+      </c>
+    </row>
+    <row r="334" spans="1:3">
+      <c r="A334" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B334">
+        <v>11</v>
+      </c>
+      <c r="C334">
+        <v>0.670447826385498</v>
+      </c>
+    </row>
+    <row r="335" spans="1:3">
+      <c r="A335" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B335">
+        <v>12</v>
+      </c>
+      <c r="C335">
+        <v>0.5710177421569824</v>
+      </c>
+    </row>
+    <row r="336" spans="1:3">
+      <c r="A336" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B336">
+        <v>13</v>
+      </c>
+      <c r="C336">
+        <v>0.4251908361911774</v>
+      </c>
+    </row>
+    <row r="337" spans="1:3">
+      <c r="A337" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B337">
+        <v>14</v>
+      </c>
+      <c r="C337">
+        <v>0.5492768287658691</v>
+      </c>
+    </row>
+    <row r="338" spans="1:3">
+      <c r="A338" s="1">
+        <v>45378</v>
+      </c>
+      <c r="B338">
+        <v>15</v>
+      </c>
+      <c r="C338">
+        <v>0.5330129861831665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying the Automation for Transavia Production
</commit_message>
<xml_diff>
--- a/Transavia/Production/Results/Results_daily_Abator_Bocsa.xlsx
+++ b/Transavia/Production/Results/Results_daily_Abator_Bocsa.xlsx
@@ -377,98 +377,98 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0.3039960861206055</v>
+        <v>0.4341971278190613</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C3">
-        <v>0.138564258813858</v>
+        <v>0.5197409987449646</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>0.007687882520258427</v>
+        <v>0.5514614582061768</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>0.0006087372894398868</v>
+        <v>0.5780135989189148</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B6">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>0.0006087372894398868</v>
+        <v>0.4727505743503571</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>0.0006087372894398868</v>
+        <v>0.3294726014137268</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>0.0006087372894398868</v>
+        <v>0.1639994531869888</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>0.0006087372894398868</v>
+        <v>0.004746152088046074</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1">
-        <v>45364</v>
+        <v>45365</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C10">
         <v>0.0006087372894398868</v>
@@ -479,10 +479,10 @@
         <v>45365</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C11">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -490,10 +490,10 @@
         <v>45365</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C12">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -501,10 +501,10 @@
         <v>45365</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C13">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -512,10 +512,10 @@
         <v>45365</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -523,18 +523,18 @@
         <v>45365</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C15">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <v>0.001462202053517103</v>
@@ -542,200 +542,200 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>0.1531635969877243</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C18">
-        <v>0.2864326238632202</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>0.3269355893135071</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B20">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>0.342717707157135</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>0.5333595275878906</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B22">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C22">
-        <v>0.6083981990814209</v>
+        <v>0.2193846851587296</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C23">
-        <v>0.5802819132804871</v>
+        <v>0.3505081832408905</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B24">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C24">
-        <v>0.5956315994262695</v>
+        <v>0.3596910238265991</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C25">
-        <v>0.4815758168697357</v>
+        <v>0.3905557096004486</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B26">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C26">
-        <v>0.3294726014137268</v>
+        <v>0.6387864947319031</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B27">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C27">
-        <v>0.1639994531869888</v>
+        <v>0.6979445815086365</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B28">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C28">
-        <v>0.008538169786334038</v>
+        <v>0.6234360933303833</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B29">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C29">
-        <v>0.0006087372894398868</v>
+        <v>0.6106366515159607</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B30">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C30">
-        <v>0.0006087372894398868</v>
+        <v>0.5007489919662476</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B31">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C31">
-        <v>0.0006087372894398868</v>
+        <v>0.4101051390171051</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B32">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C32">
-        <v>0.0006087372894398868</v>
+        <v>0.1863352507352829</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B33">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C33">
-        <v>0.0006087372894398868</v>
+        <v>0.01308351848274469</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1">
-        <v>45365</v>
+        <v>45366</v>
       </c>
       <c r="B34">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C34">
-        <v>0.0006087372894398868</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -743,10 +743,10 @@
         <v>45366</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C35">
-        <v>0.001462202053517103</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -754,10 +754,10 @@
         <v>45366</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C36">
-        <v>0.001462202053517103</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -765,10 +765,10 @@
         <v>45366</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C37">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -776,10 +776,10 @@
         <v>45366</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C38">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -787,18 +787,18 @@
         <v>45366</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C39">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <v>0.001462202053517103</v>
@@ -806,200 +806,200 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>0.2028349190950394</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C42">
-        <v>0.3505081832408905</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B43">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C43">
-        <v>0.3678479492664337</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B44">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>0.4498375952243805</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B45">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C45">
-        <v>0.6469483971595764</v>
+        <v>0.01354346703737974</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B46">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C46">
-        <v>0.6009387373924255</v>
+        <v>0.1987430304288864</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B47">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C47">
-        <v>0.6074647903442383</v>
+        <v>0.3444830477237701</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B48">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C48">
-        <v>0.6316176652908325</v>
+        <v>0.4034688174724579</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B49">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>0.5226923823356628</v>
+        <v>0.4328113496303558</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B50">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C50">
-        <v>0.4252724945545197</v>
+        <v>0.6680295467376709</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B51">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C51">
-        <v>0.1775433868169785</v>
+        <v>0.7255303859710693</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B52">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C52">
-        <v>0.01243957597762346</v>
+        <v>0.7371631860733032</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B53">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C53">
-        <v>0.001019873307086527</v>
+        <v>0.6534355878829956</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B54">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C54">
-        <v>0.0006087372894398868</v>
+        <v>0.697901725769043</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B55">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C55">
-        <v>0.0006087372894398868</v>
+        <v>0.5598261952400208</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B56">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C56">
-        <v>0.0006087372894398868</v>
+        <v>0.2996737957000732</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B57">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C57">
-        <v>0.0006087372894398868</v>
+        <v>0.01743231527507305</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1">
-        <v>45366</v>
+        <v>45367</v>
       </c>
       <c r="B58">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C58">
-        <v>0.0006087372894398868</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1007,10 +1007,10 @@
         <v>45367</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C59">
-        <v>0.001462202053517103</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1018,10 +1018,10 @@
         <v>45367</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C60">
-        <v>0.001462202053517103</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1029,10 +1029,10 @@
         <v>45367</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C61">
-        <v>0.001462202053517103</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1040,10 +1040,10 @@
         <v>45367</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C62">
-        <v>0.001462202053517103</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1051,219 +1051,219 @@
         <v>45367</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C63">
-        <v>0.001462202053517103</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C64">
-        <v>0.01354346703737974</v>
+        <v>0.001873338012956083</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B65">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C65">
-        <v>0.203892782330513</v>
+        <v>0.001873338012956083</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B66">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C66">
-        <v>0.3538053929805756</v>
+        <v>0.001873338012956083</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B67">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>0.381721556186676</v>
+        <v>0.001873338012956083</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B68">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>0.4433241784572601</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B69">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C69">
-        <v>0.6273519396781921</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B70">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C70">
-        <v>0.6669963598251343</v>
+        <v>0.1169179677963257</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C71">
-        <v>0.6575444340705872</v>
+        <v>0.250605970621109</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B72">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>0.6338027715682983</v>
+        <v>0.2961581349372864</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B73">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C73">
-        <v>0.5384136438369751</v>
+        <v>0.524865448474884</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B74">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C74">
-        <v>0.472400575876236</v>
+        <v>0.6430674195289612</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B75">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C75">
-        <v>0.2025753557682037</v>
+        <v>0.6605802178382874</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B76">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C76">
-        <v>0.01743231527507305</v>
+        <v>0.6479848027229309</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B77">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C77">
-        <v>0.001822930993512273</v>
+        <v>0.6974890828132629</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B78">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C78">
-        <v>0.001019873307086527</v>
+        <v>0.5467653870582581</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B79">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C79">
-        <v>0.001019873307086527</v>
+        <v>0.4183931052684784</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B80">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C80">
-        <v>0.001019873307086527</v>
+        <v>0.1649259477853775</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B81">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C81">
-        <v>0.001019873307086527</v>
+        <v>0.02351896092295647</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" s="1">
-        <v>45367</v>
+        <v>45368</v>
       </c>
       <c r="B82">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C82">
-        <v>0.001019873307086527</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="83" spans="1:3">
@@ -1271,10 +1271,10 @@
         <v>45368</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C83">
-        <v>0.001873338012956083</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="84" spans="1:3">
@@ -1282,10 +1282,10 @@
         <v>45368</v>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C84">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="85" spans="1:3">
@@ -1293,10 +1293,10 @@
         <v>45368</v>
       </c>
       <c r="B85">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C85">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="86" spans="1:3">
@@ -1304,10 +1304,10 @@
         <v>45368</v>
       </c>
       <c r="B86">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C86">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="87" spans="1:3">
@@ -1315,18 +1315,18 @@
         <v>45368</v>
       </c>
       <c r="B87">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C87">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B88">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C88">
         <v>0.001462202053517103</v>
@@ -1334,200 +1334,200 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B89">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C89">
-        <v>0.1169179677963257</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B90">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C90">
-        <v>0.2180894762277603</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B91">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C91">
-        <v>0.3768282532691956</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B92">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C92">
-        <v>0.5186205506324768</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B93">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C93">
-        <v>0.6430674195289612</v>
+        <v>0.01354346703737974</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B94">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C94">
-        <v>0.6727409362792969</v>
+        <v>0.2034605592489243</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B95">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C95">
-        <v>0.6742448806762695</v>
+        <v>0.325206071138382</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B96">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C96">
-        <v>0.6349566578865051</v>
+        <v>0.3994565606117249</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B97">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C97">
-        <v>0.5490165948867798</v>
+        <v>0.4333580136299133</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B98">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C98">
-        <v>0.443498969078064</v>
+        <v>0.5966976284980774</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B99">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C99">
-        <v>0.1606403440237045</v>
+        <v>0.7255303859710693</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B100">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C100">
-        <v>0.009733018465340137</v>
+        <v>0.7421822547912598</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B101">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C101">
-        <v>0.0006087372894398868</v>
+        <v>0.735063910484314</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B102">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C102">
-        <v>0.0006087372894398868</v>
+        <v>0.6510583758354187</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B103">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C103">
-        <v>0.0006087372894398868</v>
+        <v>0.6265961527824402</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B104">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C104">
-        <v>0.0006087372894398868</v>
+        <v>0.4039880335330963</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B105">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C105">
-        <v>0.0006087372894398868</v>
+        <v>0.02306810207664967</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" s="1">
-        <v>45368</v>
+        <v>45369</v>
       </c>
       <c r="B106">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C106">
-        <v>0.0006087372894398868</v>
+        <v>0.005025160033255816</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -1535,10 +1535,10 @@
         <v>45369</v>
       </c>
       <c r="B107">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C107">
-        <v>0.001462202053517103</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -1546,10 +1546,10 @@
         <v>45369</v>
       </c>
       <c r="B108">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C108">
-        <v>0.001462202053517103</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -1557,10 +1557,10 @@
         <v>45369</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C109">
-        <v>0.001462202053517103</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -1568,10 +1568,10 @@
         <v>45369</v>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C110">
-        <v>0.001462202053517103</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -1579,219 +1579,219 @@
         <v>45369</v>
       </c>
       <c r="B111">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C111">
-        <v>0.001462202053517103</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B112">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C112">
-        <v>0.01375892665237188</v>
+        <v>0.003186529269441962</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B113">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C113">
-        <v>0.219965010881424</v>
+        <v>0.003186529269441962</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B114">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C114">
-        <v>0.3492618501186371</v>
+        <v>0.003186529269441962</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B115">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C115">
-        <v>0.3729380369186401</v>
+        <v>0.001873338012956083</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B116">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>0.414051741361618</v>
+        <v>0.001582423108629882</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B117">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C117">
-        <v>0.4409171342849731</v>
+        <v>0.0172316450625658</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B118">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>0.5409641861915588</v>
+        <v>0.1193245202302933</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B119">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C119">
-        <v>0.5497909784317017</v>
+        <v>0.2565146684646606</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B120">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C120">
-        <v>0.5241569876670837</v>
+        <v>0.400177925825119</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B121">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C121">
-        <v>0.5577781796455383</v>
+        <v>0.5388127565383911</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B122">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C122">
-        <v>0.4442236423492432</v>
+        <v>0.6162009835243225</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B123">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C123">
-        <v>0.2170901447534561</v>
+        <v>0.6197966933250427</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B124">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C124">
-        <v>0.02100068144500256</v>
+        <v>0.545890212059021</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B125">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C125">
-        <v>0.001019873307086527</v>
+        <v>0.4940564632415771</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B126">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C126">
-        <v>0.001019873307086527</v>
+        <v>0.4468912780284882</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B127">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C127">
-        <v>0.0006087372894398868</v>
+        <v>0.3802532851696014</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B128">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C128">
-        <v>0.0006087372894398868</v>
+        <v>0.1856812983751297</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B129">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C129">
-        <v>0.0006087372894398868</v>
+        <v>0.01965748704969883</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" s="1">
-        <v>45369</v>
+        <v>45370</v>
       </c>
       <c r="B130">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C130">
-        <v>0.0006087372894398868</v>
+        <v>0.00233306479640305</v>
       </c>
     </row>
     <row r="131" spans="1:3">
@@ -1799,10 +1799,10 @@
         <v>45370</v>
       </c>
       <c r="B131">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C131">
-        <v>0.001462202053517103</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="132" spans="1:3">
@@ -1810,10 +1810,10 @@
         <v>45370</v>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C132">
-        <v>0.001462202053517103</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -1821,10 +1821,10 @@
         <v>45370</v>
       </c>
       <c r="B133">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C133">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="134" spans="1:3">
@@ -1832,10 +1832,10 @@
         <v>45370</v>
       </c>
       <c r="B134">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C134">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="135" spans="1:3">
@@ -1843,216 +1843,216 @@
         <v>45370</v>
       </c>
       <c r="B135">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C135">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B136">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C136">
-        <v>0.01375892665237188</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B137">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C137">
-        <v>0.1554246991872787</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B138">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C138">
-        <v>0.2826413214206696</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B139">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C139">
-        <v>0.3504942953586578</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B140">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C140">
-        <v>0.4736542999744415</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B141">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C141">
-        <v>0.6175188422203064</v>
+        <v>0.03417296335101128</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B142">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C142">
-        <v>0.55228191614151</v>
+        <v>0.1963198333978653</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B143">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C143">
-        <v>0.77106773853302</v>
+        <v>0.3272940218448639</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B144">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C144">
-        <v>0.7280515432357788</v>
+        <v>0.3496451377868652</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B145">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C145">
-        <v>0.6689601540565491</v>
+        <v>0.4450734853744507</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B146">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C146">
-        <v>0.5792936682701111</v>
+        <v>0.6078290939331055</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B147">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C147">
-        <v>0.3157016336917877</v>
+        <v>0.6636301875114441</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B148">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C148">
-        <v>0.02100843377411366</v>
+        <v>0.6386595368385315</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B149">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C149">
-        <v>0.005535293836146593</v>
+        <v>0.6141873598098755</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B150">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C150">
-        <v>0.00233306479640305</v>
+        <v>0.4568880200386047</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B151">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C151">
-        <v>0.00233306479640305</v>
+        <v>0.4248524308204651</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B152">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C152">
-        <v>0.00233306479640305</v>
+        <v>0.1957428306341171</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B153">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C153">
-        <v>0.001019873307086527</v>
+        <v>0.02025477215647697</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" s="1">
-        <v>45370</v>
+        <v>45371</v>
       </c>
       <c r="B154">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C154">
         <v>0.001019873307086527</v>
@@ -2063,10 +2063,10 @@
         <v>45371</v>
       </c>
       <c r="B155">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C155">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="156" spans="1:3">
@@ -2074,10 +2074,10 @@
         <v>45371</v>
       </c>
       <c r="B156">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C156">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="157" spans="1:3">
@@ -2085,10 +2085,10 @@
         <v>45371</v>
       </c>
       <c r="B157">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C157">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="158" spans="1:3">
@@ -2096,10 +2096,10 @@
         <v>45371</v>
       </c>
       <c r="B158">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C158">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="159" spans="1:3">
@@ -2107,219 +2107,219 @@
         <v>45371</v>
       </c>
       <c r="B159">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C159">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B160">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C160">
-        <v>0.0144943306222558</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B161">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C161">
-        <v>0.1657159030437469</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B162">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C162">
-        <v>0.3122064471244812</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B163">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C163">
-        <v>0.3471722900867462</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B164">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C164">
-        <v>0.502892792224884</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B165">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C165">
-        <v>0.5648559927940369</v>
+        <v>0.04184490442276001</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B166">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C166">
-        <v>0.7599678635597229</v>
+        <v>0.2407538443803787</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B167">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C167">
-        <v>0.7935822010040283</v>
+        <v>0.3205101788043976</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B168">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C168">
-        <v>0.8243045210838318</v>
+        <v>0.4004832804203033</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B169">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C169">
-        <v>0.7576906085014343</v>
+        <v>0.4344783127307892</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B170">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C170">
-        <v>0.614687979221344</v>
+        <v>0.6392068266868591</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B171">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C171">
-        <v>0.3211678862571716</v>
+        <v>0.7444438934326172</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B172">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C172">
-        <v>0.02528130449354649</v>
+        <v>0.7098835706710815</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B173">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C173">
-        <v>0.004636262077838182</v>
+        <v>0.7434342503547668</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B174">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C174">
-        <v>0.001560923759825528</v>
+        <v>0.6908097863197327</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B175">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C175">
-        <v>0.001560923759825528</v>
+        <v>0.5798523426055908</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B176">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C176">
-        <v>0.001822930993512273</v>
+        <v>0.3213266730308533</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B177">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C177">
-        <v>0.001822930993512273</v>
+        <v>0.02528130449354649</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" s="1">
-        <v>45371</v>
+        <v>45372</v>
       </c>
       <c r="B178">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C178">
-        <v>0.001822930993512273</v>
+        <v>0.005025160033255816</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -2327,10 +2327,10 @@
         <v>45372</v>
       </c>
       <c r="B179">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C179">
-        <v>0.001873338012956083</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -2338,10 +2338,10 @@
         <v>45372</v>
       </c>
       <c r="B180">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C180">
-        <v>0.001873338012956083</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -2349,10 +2349,10 @@
         <v>45372</v>
       </c>
       <c r="B181">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C181">
-        <v>0.001873338012956083</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -2360,10 +2360,10 @@
         <v>45372</v>
       </c>
       <c r="B182">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C182">
-        <v>0.001873338012956083</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -2371,219 +2371,219 @@
         <v>45372</v>
       </c>
       <c r="B183">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C183">
-        <v>0.001873338012956083</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B184">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C184">
-        <v>0.04279576241970062</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B185">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C185">
-        <v>0.2264294177293777</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B186">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C186">
-        <v>0.3320692181587219</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B187">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C187">
-        <v>0.3862507045269012</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B188">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C188">
-        <v>0.447108268737793</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B189">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C189">
-        <v>0.7802374362945557</v>
+        <v>0.04279576241970062</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B190">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C190">
-        <v>0.821527898311615</v>
+        <v>0.1924201846122742</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B191">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C191">
-        <v>0.8387635946273804</v>
+        <v>0.3695197403430939</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B192">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C192">
-        <v>0.7663832902908325</v>
+        <v>0.3798917531967163</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B193">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C193">
-        <v>0.6836625933647156</v>
+        <v>0.4777755737304688</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B194">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C194">
-        <v>0.6602174639701843</v>
+        <v>0.6030239462852478</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B195">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C195">
-        <v>0.3830647766590118</v>
+        <v>0.720662534236908</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B196">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C196">
-        <v>0.02511965297162533</v>
+        <v>0.8306076526641846</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B197">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C197">
-        <v>0.004636262077838182</v>
+        <v>0.8135381937026978</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B198">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C198">
-        <v>0.001560923759825528</v>
+        <v>0.7103910446166992</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B199">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C199">
-        <v>0.001560923759825528</v>
+        <v>0.6176931262016296</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B200">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C200">
-        <v>0.001560923759825528</v>
+        <v>0.3304107189178467</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B201">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C201">
-        <v>0.001560923759825528</v>
+        <v>0.02521934546530247</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" s="1">
-        <v>45372</v>
+        <v>45373</v>
       </c>
       <c r="B202">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C202">
-        <v>0.001560923759825528</v>
+        <v>0.005025160033255816</v>
       </c>
     </row>
     <row r="203" spans="1:3">
@@ -2591,10 +2591,10 @@
         <v>45373</v>
       </c>
       <c r="B203">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C203">
-        <v>0.002426850143820047</v>
+        <v>0.001822930993512273</v>
       </c>
     </row>
     <row r="204" spans="1:3">
@@ -2602,10 +2602,10 @@
         <v>45373</v>
       </c>
       <c r="B204">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C204">
-        <v>0.002426850143820047</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="205" spans="1:3">
@@ -2613,10 +2613,10 @@
         <v>45373</v>
       </c>
       <c r="B205">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C205">
-        <v>0.002426850143820047</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="206" spans="1:3">
@@ -2624,10 +2624,10 @@
         <v>45373</v>
       </c>
       <c r="B206">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C206">
-        <v>0.002676395466551185</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="207" spans="1:3">
@@ -2635,219 +2635,219 @@
         <v>45373</v>
       </c>
       <c r="B207">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C207">
-        <v>0.002676395466551185</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B208">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C208">
-        <v>0.04334927350282669</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B209">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C209">
-        <v>0.201739564538002</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B210">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C210">
-        <v>0.3197154104709625</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B211">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C211">
-        <v>0.3832141160964966</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B212">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C212">
-        <v>0.4454418122768402</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B213">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C213">
-        <v>0.6977189779281616</v>
+        <v>0.04206036403775215</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B214">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C214">
-        <v>0.7818703055381775</v>
+        <v>0.1893366426229477</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B215">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C215">
-        <v>0.7823619246482849</v>
+        <v>0.3303806483745575</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B216">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C216">
-        <v>0.9103758931159973</v>
+        <v>0.3740314245223999</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B217">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C217">
-        <v>0.7971689701080322</v>
+        <v>0.5296344757080078</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B218">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C218">
-        <v>0.7029615044593811</v>
+        <v>0.6621710658073425</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B219">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C219">
-        <v>0.511029839515686</v>
+        <v>0.6962389349937439</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B220">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C220">
-        <v>0.03001339919865131</v>
+        <v>0.7080342173576355</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B221">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C221">
-        <v>0.006026065442711115</v>
+        <v>0.7134918570518494</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B222">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C222">
-        <v>-0.001574540045112371</v>
+        <v>0.6088898777961731</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B223">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C223">
-        <v>-0.001574540045112371</v>
+        <v>0.5358288288116455</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B224">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C224">
-        <v>-0.003064034273847938</v>
+        <v>0.2616091370582581</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B225">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C225">
-        <v>-0.003064034273847938</v>
+        <v>0.03214943036437035</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="1">
-        <v>45373</v>
+        <v>45374</v>
       </c>
       <c r="B226">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C226">
-        <v>0.001560923759825528</v>
+        <v>0.0009648292907513678</v>
       </c>
     </row>
     <row r="227" spans="1:3">
@@ -2855,10 +2855,10 @@
         <v>45374</v>
       </c>
       <c r="B227">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C227">
-        <v>0.002426850143820047</v>
+        <v>0.0005536933313123882</v>
       </c>
     </row>
     <row r="228" spans="1:3">
@@ -2866,10 +2866,10 @@
         <v>45374</v>
       </c>
       <c r="B228">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C228">
-        <v>0.002426850143820047</v>
+        <v>0.0005536933313123882</v>
       </c>
     </row>
     <row r="229" spans="1:3">
@@ -2877,10 +2877,10 @@
         <v>45374</v>
       </c>
       <c r="B229">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C229">
-        <v>0.002426850143820047</v>
+        <v>0.0005536933313123882</v>
       </c>
     </row>
     <row r="230" spans="1:3">
@@ -2888,10 +2888,10 @@
         <v>45374</v>
       </c>
       <c r="B230">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C230">
-        <v>0.002676395466551185</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -2899,219 +2899,219 @@
         <v>45374</v>
       </c>
       <c r="B231">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C231">
-        <v>0.002936984179541469</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B232">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C232">
-        <v>0.03597201034426689</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B233">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C233">
-        <v>0.1678444594144821</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B234">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C234">
-        <v>0.2831286489963531</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B235">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C235">
-        <v>0.3570091128349304</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B236">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C236">
-        <v>0.5389638543128967</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B237">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C237">
-        <v>0.7659305930137634</v>
+        <v>0.04184490442276001</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B238">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C238">
-        <v>0.838615894317627</v>
+        <v>0.2247408181428909</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B239">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C239">
-        <v>0.8198053240776062</v>
+        <v>0.3142106831073761</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B240">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C240">
-        <v>0.840302050113678</v>
+        <v>0.3179850876331329</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B241">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C241">
-        <v>0.7809241414070129</v>
+        <v>0.4620073735713959</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B242">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C242">
-        <v>0.563556432723999</v>
+        <v>0.582944929599762</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B243">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C243">
-        <v>0.3210353851318359</v>
+        <v>0.5905654430389404</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B244">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C244">
-        <v>0.02221535332500935</v>
+        <v>0.6041321158409119</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B245">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C245">
-        <v>0.004636262077838182</v>
+        <v>0.6106366515159607</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B246">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C246">
-        <v>0.001560923759825528</v>
+        <v>0.5188617706298828</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B247">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C247">
-        <v>0.001560923759825528</v>
+        <v>0.4614161849021912</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B248">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C248">
-        <v>0.001560923759825528</v>
+        <v>0.2020462602376938</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B249">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C249">
-        <v>0.002071057911962271</v>
+        <v>0.02345700189471245</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" s="1">
-        <v>45374</v>
+        <v>45375</v>
       </c>
       <c r="B250">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C250">
-        <v>0.002071057911962271</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="251" spans="1:3">
@@ -3119,10 +3119,10 @@
         <v>45375</v>
       </c>
       <c r="B251">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C251">
-        <v>0.003186529269441962</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="252" spans="1:3">
@@ -3130,10 +3130,10 @@
         <v>45375</v>
       </c>
       <c r="B252">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C252">
-        <v>0.003186529269441962</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="253" spans="1:3">
@@ -3141,10 +3141,10 @@
         <v>45375</v>
       </c>
       <c r="B253">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C253">
-        <v>0.003186529269441962</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="254" spans="1:3">
@@ -3152,10 +3152,10 @@
         <v>45375</v>
       </c>
       <c r="B254">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C254">
-        <v>0.003186529269441962</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="255" spans="1:3">
@@ -3163,219 +3163,219 @@
         <v>45375</v>
       </c>
       <c r="B255">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C255">
-        <v>0.003186529269441962</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B256">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C256">
-        <v>0.03793659061193466</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B257">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C257">
-        <v>0.1589391231536865</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B258">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C258">
-        <v>0.2691071033477783</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B259">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C259">
-        <v>0.3982172310352325</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B260">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C260">
-        <v>0.5408667325973511</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B261">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C261">
-        <v>0.6022312045097351</v>
+        <v>0.06855346262454987</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B262">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C262">
-        <v>0.7723228335380554</v>
+        <v>0.2750999629497528</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B263">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C263">
-        <v>0.7553914785385132</v>
+        <v>0.3401879370212555</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B264">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C264">
-        <v>0.780234158039093</v>
+        <v>0.3613895177841187</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B265">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C265">
-        <v>0.6081504821777344</v>
+        <v>0.5289963483810425</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B266">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C266">
-        <v>0.5824326872825623</v>
+        <v>0.5941035747528076</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B267">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C267">
-        <v>0.3905293047428131</v>
+        <v>0.6724932789802551</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B268">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C268">
-        <v>0.02817033790051937</v>
+        <v>0.6460258364677429</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B269">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C269">
-        <v>0.005025160033255816</v>
+        <v>0.6203449368476868</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B270">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C270">
-        <v>0.001560923759825528</v>
+        <v>0.5244210958480835</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B271">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C271">
-        <v>0.00233306479640305</v>
+        <v>0.4517869353294373</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B272">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C272">
-        <v>0.001019873307086527</v>
+        <v>0.1564520597457886</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B273">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C273">
-        <v>0.001019873307086527</v>
+        <v>0.01047892775386572</v>
       </c>
     </row>
     <row r="274" spans="1:3">
       <c r="A274" s="1">
-        <v>45375</v>
+        <v>45376</v>
       </c>
       <c r="B274">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C274">
-        <v>0.001019873307086527</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="275" spans="1:3">
@@ -3383,10 +3383,10 @@
         <v>45376</v>
       </c>
       <c r="B275">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C275">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="276" spans="1:3">
@@ -3394,10 +3394,10 @@
         <v>45376</v>
       </c>
       <c r="B276">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C276">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="277" spans="1:3">
@@ -3405,10 +3405,10 @@
         <v>45376</v>
       </c>
       <c r="B277">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C277">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="278" spans="1:3">
@@ -3416,10 +3416,10 @@
         <v>45376</v>
       </c>
       <c r="B278">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C278">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="279" spans="1:3">
@@ -3427,219 +3427,219 @@
         <v>45376</v>
       </c>
       <c r="B279">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C279">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B280">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C280">
-        <v>0.08701945096254349</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B281">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C281">
-        <v>0.296549379825592</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B282">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C282">
-        <v>0.3118192553520203</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B283">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C283">
-        <v>0.2224577516317368</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B284">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C284">
-        <v>0.4194476008415222</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B285">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C285">
-        <v>0.5621249675750732</v>
+        <v>0.07283658534288406</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B286">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C286">
-        <v>0.6006543636322021</v>
+        <v>0.2762148678302765</v>
       </c>
     </row>
     <row r="287" spans="1:3">
       <c r="A287" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B287">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C287">
-        <v>0.7866647839546204</v>
+        <v>0.3559424877166748</v>
       </c>
     </row>
     <row r="288" spans="1:3">
       <c r="A288" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B288">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C288">
-        <v>0.7469737529754639</v>
+        <v>0.3460376858711243</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="A289" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B289">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C289">
-        <v>0.7285200357437134</v>
+        <v>0.367854505777359</v>
       </c>
     </row>
     <row r="290" spans="1:3">
       <c r="A290" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B290">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C290">
-        <v>0.6659958958625793</v>
+        <v>0.621116578578949</v>
       </c>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B291">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C291">
-        <v>0.4039880335330963</v>
+        <v>0.6441700458526611</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B292">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C292">
-        <v>0.03032158501446247</v>
+        <v>0.4535526931285858</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B293">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C293">
-        <v>0.005025160033255816</v>
+        <v>0.4512429535388947</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B294">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C294">
-        <v>0.001822930993512273</v>
+        <v>0.4873920381069183</v>
       </c>
     </row>
     <row r="295" spans="1:3">
       <c r="A295" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B295">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C295">
-        <v>0.001822930993512273</v>
+        <v>0.4591299593448639</v>
       </c>
     </row>
     <row r="296" spans="1:3">
       <c r="A296" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B296">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C296">
-        <v>0.001019873307086527</v>
+        <v>0.2511695027351379</v>
       </c>
     </row>
     <row r="297" spans="1:3">
       <c r="A297" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B297">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C297">
-        <v>0.001019873307086527</v>
+        <v>0.02835137769579887</v>
       </c>
     </row>
     <row r="298" spans="1:3">
       <c r="A298" s="1">
-        <v>45376</v>
+        <v>45377</v>
       </c>
       <c r="B298">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C298">
-        <v>0.001019873307086527</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="299" spans="1:3">
@@ -3647,10 +3647,10 @@
         <v>45377</v>
       </c>
       <c r="B299">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C299">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="300" spans="1:3">
@@ -3658,10 +3658,10 @@
         <v>45377</v>
       </c>
       <c r="B300">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C300">
-        <v>0.001873338012956083</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="301" spans="1:3">
@@ -3669,10 +3669,10 @@
         <v>45377</v>
       </c>
       <c r="B301">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C301">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="302" spans="1:3">
@@ -3680,10 +3680,10 @@
         <v>45377</v>
       </c>
       <c r="B302">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C302">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="303" spans="1:3">
@@ -3691,219 +3691,219 @@
         <v>45377</v>
       </c>
       <c r="B303">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C303">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="304" spans="1:3">
       <c r="A304" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B304">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C304">
-        <v>0.04206036403775215</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="305" spans="1:3">
       <c r="A305" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B305">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C305">
-        <v>0.181069627404213</v>
+        <v>0.001190799288451672</v>
       </c>
     </row>
     <row r="306" spans="1:3">
       <c r="A306" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B306">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C306">
-        <v>0.3110060691833496</v>
+        <v>0.001190799288451672</v>
       </c>
     </row>
     <row r="307" spans="1:3">
       <c r="A307" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B307">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C307">
-        <v>0.3256857991218567</v>
+        <v>0.001190799288451672</v>
       </c>
     </row>
     <row r="308" spans="1:3">
       <c r="A308" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B308">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C308">
-        <v>0.4600401222705841</v>
+        <v>0.001190799288451672</v>
       </c>
     </row>
     <row r="309" spans="1:3">
       <c r="A309" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B309">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C309">
-        <v>0.5852345824241638</v>
+        <v>0.08555274456739426</v>
       </c>
     </row>
     <row r="310" spans="1:3">
       <c r="A310" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B310">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C310">
-        <v>0.5273016095161438</v>
+        <v>0.2852441668510437</v>
       </c>
     </row>
     <row r="311" spans="1:3">
       <c r="A311" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B311">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C311">
-        <v>0.6154138445854187</v>
+        <v>0.3280532956123352</v>
       </c>
     </row>
     <row r="312" spans="1:3">
       <c r="A312" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B312">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C312">
-        <v>0.6494281888008118</v>
+        <v>0.2335449159145355</v>
       </c>
     </row>
     <row r="313" spans="1:3">
       <c r="A313" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B313">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C313">
-        <v>0.5516771674156189</v>
+        <v>0.4718027710914612</v>
       </c>
     </row>
     <row r="314" spans="1:3">
       <c r="A314" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B314">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C314">
-        <v>0.4223678410053253</v>
+        <v>0.510876476764679</v>
       </c>
     </row>
     <row r="315" spans="1:3">
       <c r="A315" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B315">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C315">
-        <v>0.1634838283061981</v>
+        <v>0.5512218475341797</v>
       </c>
     </row>
     <row r="316" spans="1:3">
       <c r="A316" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B316">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C316">
-        <v>0.009733018465340137</v>
+        <v>0.5007044076919556</v>
       </c>
     </row>
     <row r="317" spans="1:3">
       <c r="A317" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B317">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C317">
-        <v>0.0006087372894398868</v>
+        <v>0.3306083679199219</v>
       </c>
     </row>
     <row r="318" spans="1:3">
       <c r="A318" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B318">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C318">
-        <v>0.0006087372894398868</v>
+        <v>0.5076180696487427</v>
       </c>
     </row>
     <row r="319" spans="1:3">
       <c r="A319" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B319">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C319">
-        <v>0.0006087372894398868</v>
+        <v>0.4830609858036041</v>
       </c>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B320">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C320">
-        <v>0.0006087372894398868</v>
+        <v>0.2733346521854401</v>
       </c>
     </row>
     <row r="321" spans="1:3">
       <c r="A321" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B321">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C321">
-        <v>0.0006087372894398868</v>
+        <v>0.02915443480014801</v>
       </c>
     </row>
     <row r="322" spans="1:3">
       <c r="A322" s="1">
-        <v>45377</v>
+        <v>45378</v>
       </c>
       <c r="B322">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C322">
-        <v>0.0006087372894398868</v>
+        <v>0.001019873307086527</v>
       </c>
     </row>
     <row r="323" spans="1:3">
@@ -3911,10 +3911,10 @@
         <v>45378</v>
       </c>
       <c r="B323">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C323">
-        <v>0.001462202053517103</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="324" spans="1:3">
@@ -3922,10 +3922,10 @@
         <v>45378</v>
       </c>
       <c r="B324">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C324">
-        <v>0.001190799288451672</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="325" spans="1:3">
@@ -3933,10 +3933,10 @@
         <v>45378</v>
       </c>
       <c r="B325">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C325">
-        <v>0.001190799288451672</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="326" spans="1:3">
@@ -3944,10 +3944,10 @@
         <v>45378</v>
       </c>
       <c r="B326">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C326">
-        <v>0.001190799288451672</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="327" spans="1:3">
@@ -3955,131 +3955,131 @@
         <v>45378</v>
       </c>
       <c r="B327">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="C327">
-        <v>0.001190799288451672</v>
+        <v>0.0006087372894398868</v>
       </c>
     </row>
     <row r="328" spans="1:3">
       <c r="A328" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B328">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C328">
-        <v>0.08555274456739426</v>
+        <v>0.001462202053517103</v>
       </c>
     </row>
     <row r="329" spans="1:3">
       <c r="A329" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B329">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C329">
-        <v>0.2255028635263443</v>
+        <v>0.001190799288451672</v>
       </c>
     </row>
     <row r="330" spans="1:3">
       <c r="A330" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B330">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C330">
-        <v>0.3339379131793976</v>
+        <v>0.001190799288451672</v>
       </c>
     </row>
     <row r="331" spans="1:3">
       <c r="A331" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B331">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C331">
-        <v>0.2840148508548737</v>
+        <v>0.001190799288451672</v>
       </c>
     </row>
     <row r="332" spans="1:3">
       <c r="A332" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B332">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C332">
-        <v>0.609189510345459</v>
+        <v>0.001190799288451672</v>
       </c>
     </row>
     <row r="333" spans="1:3">
       <c r="A333" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B333">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C333">
-        <v>0.6064830422401428</v>
+        <v>0.1045091971755028</v>
       </c>
     </row>
     <row r="334" spans="1:3">
       <c r="A334" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B334">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C334">
-        <v>0.670447826385498</v>
+        <v>0.2904259264469147</v>
       </c>
     </row>
     <row r="335" spans="1:3">
       <c r="A335" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B335">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C335">
-        <v>0.5710177421569824</v>
+        <v>0.2585297822952271</v>
       </c>
     </row>
     <row r="336" spans="1:3">
       <c r="A336" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B336">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C336">
-        <v>0.4251908361911774</v>
+        <v>0.2849051058292389</v>
       </c>
     </row>
     <row r="337" spans="1:3">
       <c r="A337" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B337">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C337">
-        <v>0.5492768287658691</v>
+        <v>0.2783945798873901</v>
       </c>
     </row>
     <row r="338" spans="1:3">
       <c r="A338" s="1">
-        <v>45378</v>
+        <v>45379</v>
       </c>
       <c r="B338">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C338">
-        <v>0.5330129861831665</v>
+        <v>0.5944923758506775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>